<commit_message>
analysis and figure done for LAR temp tech memo
</commit_message>
<xml_diff>
--- a/input_data/Temperature/Heal the Bay Temperature Logging Coordinates Dates.xlsx
+++ b/input_data/Temperature/Heal the Bay Temperature Logging Coordinates Dates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katieirving/Documents/Documents - Katie’s MacBook Pro/git/SGR_Temp_Benthic/input_data/Temperature/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B2F07FC-2453-6141-B5A0-E356D053A4B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467B515B-CDFE-E14C-91D7-51AB175C7B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38480" yWindow="7360" windowWidth="33300" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38480" yWindow="620" windowWidth="33300" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,13 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
-  <si>
-    <t>Rio Hondo Confluence</t>
-  </si>
-  <si>
-    <t>Compton Creek Confluence</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>Willow Street</t>
   </si>
@@ -76,9 +70,6 @@
     <t>Logger</t>
   </si>
   <si>
-    <t>21150075 (washed away)</t>
-  </si>
-  <si>
     <t>Start Date</t>
   </si>
   <si>
@@ -88,13 +79,34 @@
     <t xml:space="preserve">start date </t>
   </si>
   <si>
-    <t>data Gap</t>
-  </si>
-  <si>
     <t>51 days</t>
   </si>
   <si>
     <t>204 days</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>riparian</t>
+  </si>
+  <si>
+    <t>some green</t>
+  </si>
+  <si>
+    <t>eddies, trees</t>
+  </si>
+  <si>
+    <t>Natural</t>
+  </si>
+  <si>
+    <t>Concrete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21150075/21150070* </t>
+  </si>
+  <si>
+    <t>Data Gap</t>
   </si>
 </sst>
 </file>
@@ -136,7 +148,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -175,42 +187,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -224,9 +205,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -244,12 +222,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -534,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="J8" sqref="A2:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -548,233 +520,227 @@
     <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="6">
+        <v>34.170450000000002</v>
+      </c>
+      <c r="C2" s="7">
+        <v>-118.47727</v>
+      </c>
+      <c r="D2" s="9">
+        <v>21150068</v>
+      </c>
+      <c r="E2" s="14">
+        <v>44428</v>
+      </c>
+      <c r="F2" s="14">
+        <v>44489</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4">
+        <v>34.108240000000002</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-118.25251</v>
+      </c>
+      <c r="D3" s="8">
+        <v>21150077</v>
+      </c>
+      <c r="E3" s="14">
+        <v>44428</v>
+      </c>
+      <c r="F3" s="14">
+        <v>44530</v>
+      </c>
+      <c r="G3" s="14">
+        <v>44581</v>
+      </c>
+      <c r="H3" s="14">
+        <v>44711</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6">
+        <v>34.101120000000002</v>
+      </c>
+      <c r="C4" s="7">
+        <v>-118.24217</v>
+      </c>
+      <c r="D4" s="5">
+        <v>21150073</v>
+      </c>
+      <c r="E4" s="14">
+        <v>44428</v>
+      </c>
+      <c r="F4" s="14">
+        <v>44530</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="B5" s="4">
+        <v>34.0869</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-118.22796</v>
+      </c>
+      <c r="D5" s="8">
+        <v>21150074</v>
+      </c>
+      <c r="E5" s="14">
+        <v>44428</v>
+      </c>
+      <c r="F5" s="14">
+        <v>44530</v>
+      </c>
+      <c r="J5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="11">
+        <v>33.842660000000002</v>
+      </c>
+      <c r="C6" s="12">
+        <v>-118.2052</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="14">
+        <v>44428</v>
+      </c>
+      <c r="F6" s="14">
+        <v>44468</v>
+      </c>
+      <c r="G6" s="14">
+        <v>44672</v>
+      </c>
+      <c r="H6" s="14">
+        <v>44712</v>
+      </c>
+      <c r="I6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
+      <c r="J6" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="6">
+        <v>33.985849999999999</v>
+      </c>
+      <c r="C7" s="7">
+        <v>-118.17122000000001</v>
+      </c>
+      <c r="D7" s="5">
+        <v>21150065</v>
+      </c>
+      <c r="E7" s="14">
+        <v>44672</v>
+      </c>
+      <c r="F7" s="14">
+        <v>44687</v>
+      </c>
+      <c r="J7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7">
-        <v>33.931440000000002</v>
-      </c>
-      <c r="C2" s="8">
-        <v>-118.17586</v>
-      </c>
-      <c r="D2" s="5">
-        <v>21150063</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7">
-        <v>33.841410000000003</v>
-      </c>
-      <c r="C3" s="8">
-        <v>-118.20362</v>
-      </c>
-      <c r="D3" s="5">
-        <v>21150071</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4">
+      <c r="B8" s="4">
         <v>33.804679999999998</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C8" s="1">
         <v>-118.20547999999999</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D8" s="8">
         <v>21150064</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E8" s="14">
         <v>44672</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F8" s="14">
         <v>44712</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="7">
-        <v>33.985849999999999</v>
-      </c>
-      <c r="C5" s="8">
-        <v>-118.17122000000001</v>
-      </c>
-      <c r="D5" s="5">
-        <v>21150065</v>
-      </c>
-      <c r="E5" s="19">
-        <v>44672</v>
-      </c>
-      <c r="F5" s="19">
-        <v>44687</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="12">
-        <v>33.842660000000002</v>
-      </c>
-      <c r="C6" s="13">
-        <v>-118.2052</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="19">
-        <v>44428</v>
-      </c>
-      <c r="F6" s="19">
-        <v>44468</v>
-      </c>
-      <c r="G6" s="19">
-        <v>44672</v>
-      </c>
-      <c r="H6" s="19">
-        <v>44712</v>
-      </c>
-      <c r="I6" s="20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="18">
-        <v>21150070</v>
-      </c>
-      <c r="E7" s="19">
-        <v>44672</v>
-      </c>
-      <c r="F7" s="19">
-        <v>44712</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="4">
-        <v>34.0869</v>
-      </c>
-      <c r="C8" s="1">
-        <v>-118.22796</v>
-      </c>
-      <c r="D8" s="9">
-        <v>21150074</v>
-      </c>
-      <c r="E8" s="19">
-        <v>44428</v>
-      </c>
-      <c r="F8" s="19">
-        <v>44530</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="7">
-        <v>34.101120000000002</v>
-      </c>
-      <c r="C9" s="8">
-        <v>-118.24217</v>
-      </c>
-      <c r="D9" s="5">
-        <v>21150073</v>
-      </c>
-      <c r="E9" s="19">
-        <v>44428</v>
-      </c>
-      <c r="F9" s="19">
-        <v>44530</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="4">
-        <v>34.108240000000002</v>
-      </c>
-      <c r="C10" s="1">
-        <v>-118.25251</v>
-      </c>
-      <c r="D10" s="9">
-        <v>21150077</v>
-      </c>
-      <c r="E10" s="19">
-        <v>44428</v>
-      </c>
-      <c r="F10" s="19">
-        <v>44530</v>
-      </c>
-      <c r="G10" s="19">
-        <v>44581</v>
-      </c>
-      <c r="H10" s="19">
-        <v>44711</v>
-      </c>
-      <c r="I10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="7">
-        <v>34.170450000000002</v>
-      </c>
-      <c r="C11" s="8">
-        <v>-118.47727</v>
-      </c>
-      <c r="D11" s="10">
-        <v>21150068</v>
-      </c>
-      <c r="E11" s="19">
-        <v>44428</v>
-      </c>
-      <c r="F11" s="19">
-        <v>44489</v>
+      <c r="J8" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>